<commit_message>
Increase strength to Weekly Fights for Purgatories Cave of Memories, allow them to drop cosmics, information changes
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/weekly-monsters-purgatory.xlsx
+++ b/resources/data-imports/Monsters/weekly-monsters-purgatory.xlsx
@@ -175,7 +175,7 @@
     <t xml:space="preserve">Chainbound Warden</t>
   </si>
   <si>
-    <t xml:space="preserve">1622389-4431438</t>
+    <t xml:space="preserve">795381477075-997181360106</t>
   </si>
   <si>
     <t xml:space="preserve">Purgatory</t>
@@ -184,37 +184,37 @@
     <t xml:space="preserve">Soul-Flayed Prophet</t>
   </si>
   <si>
-    <t xml:space="preserve">2066486-5385877</t>
+    <t xml:space="preserve">819091798906-1021643614923</t>
   </si>
   <si>
     <t xml:space="preserve">The Shackled Flame</t>
   </si>
   <si>
-    <t xml:space="preserve">2632147-6545881</t>
+    <t xml:space="preserve">843508925432-1046705963099</t>
   </si>
   <si>
     <t xml:space="preserve">Whispers of the Chained</t>
   </si>
   <si>
-    <t xml:space="preserve">3352646-7955727</t>
+    <t xml:space="preserve">868653926499-1072383125762</t>
   </si>
   <si>
     <t xml:space="preserve">Tormentor of Twilight</t>
   </si>
   <si>
-    <t xml:space="preserve">4270367-9669224</t>
+    <t xml:space="preserve">894548500048-1098690185173</t>
   </si>
   <si>
     <t xml:space="preserve">Sorrow-Eater</t>
   </si>
   <si>
-    <t xml:space="preserve">5439297-11751771</t>
+    <t xml:space="preserve">921214990834-1125642593582</t>
   </si>
   <si>
     <t xml:space="preserve">Iron Veil Sentinel</t>
   </si>
   <si>
-    <t xml:space="preserve">6928199-14282856</t>
+    <t xml:space="preserve">948676409711-1153256182302</t>
   </si>
   <si>
     <t xml:space="preserve">Flask of ever lasting water</t>
@@ -223,25 +223,25 @@
     <t xml:space="preserve">The Miseric Executor</t>
   </si>
   <si>
-    <t xml:space="preserve">8824659-17359084</t>
+    <t xml:space="preserve">976956453484-1181547171012</t>
   </si>
   <si>
     <t xml:space="preserve">Bearer of Endless Chains</t>
   </si>
   <si>
-    <t xml:space="preserve">11240237-21097866</t>
+    <t xml:space="preserve">1006079525363-1210532177283</t>
   </si>
   <si>
     <t xml:space="preserve">Harbinger of Penance</t>
   </si>
   <si>
-    <t xml:space="preserve">14317033-25641903</t>
+    <t xml:space="preserve">1036070756014-1240228226337</t>
   </si>
   <si>
     <t xml:space="preserve">The Screaming Shade</t>
   </si>
   <si>
-    <t xml:space="preserve">18236041-31164631</t>
+    <t xml:space="preserve">1066956025251-1270652761049</t>
   </si>
   <si>
     <t xml:space="preserve">Wild Game Meat</t>
@@ -250,25 +250,25 @@
     <t xml:space="preserve">Echo of the Guilty</t>
   </si>
   <si>
-    <t xml:space="preserve">23227802-37876838</t>
+    <t xml:space="preserve">1098761984363-1301823652191</t>
   </si>
   <si>
     <t xml:space="preserve">Gravebinder of the Lost</t>
   </si>
   <si>
-    <t xml:space="preserve">29585960-46034713</t>
+    <t xml:space="preserve">1131516079117-1333759208933</t>
   </si>
   <si>
     <t xml:space="preserve">Tethered Soul Harvester</t>
   </si>
   <si>
-    <t xml:space="preserve">37684540-55949624</t>
+    <t xml:space="preserve">1165246573436-1366478189591</t>
   </si>
   <si>
     <t xml:space="preserve">Memory Eater</t>
   </si>
   <si>
-    <t xml:space="preserve">47999948-67999998</t>
+    <t xml:space="preserve">1199982573790-1399999812651</t>
   </si>
   <si>
     <t xml:space="preserve">Flame of the Prince</t>
@@ -582,16 +582,17 @@
   </sheetPr>
   <dimension ref="A1:AX16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AL1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM13" activeCellId="0" sqref="AM13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AP1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL2" activeCellId="0" sqref="AL2:AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="1" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.54"/>
@@ -605,8 +606,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="27.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="26.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="36.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="34.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="15.71"/>
@@ -789,40 +790,40 @@
         <v>50</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="K2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="P2" s="1" t="n">
         <v>0</v>
@@ -840,7 +841,7 @@
         <v>4</v>
       </c>
       <c r="U2" s="3" t="n">
-        <v>102.791747912832</v>
+        <v>497.23410416805</v>
       </c>
       <c r="V2" s="1" t="n">
         <v>0.015955343603399</v>
@@ -858,22 +859,22 @@
         <v>51</v>
       </c>
       <c r="AA2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="AB2" s="3" t="n">
-        <v>950713788.21552</v>
+        <v>618134971114.325</v>
       </c>
       <c r="AC2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="AD2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="AE2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="AF2" s="1" t="n">
-        <v>0.56429064020628</v>
+        <v>0.71857144490625</v>
       </c>
       <c r="AG2" s="1" t="n">
         <v>0.128641962097936</v>
@@ -882,16 +883,16 @@
         <v>0.128641962097936</v>
       </c>
       <c r="AI2" s="1" t="n">
-        <v>0.09927852144338</v>
+        <v>0.281716102899423</v>
       </c>
       <c r="AJ2" s="1" t="n">
-        <v>0.09927852144338</v>
+        <v>0.281716102899423</v>
       </c>
       <c r="AK2" s="1" t="n">
-        <v>0.09927852144338</v>
+        <v>0.281716102899423</v>
       </c>
       <c r="AL2" s="1" t="n">
-        <v>0.09927852144338</v>
+        <v>0.281716102899423</v>
       </c>
       <c r="AN2" s="1" t="n">
         <v>0</v>
@@ -914,40 +915,40 @@
         <v>53</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>0</v>
@@ -965,7 +966,7 @@
         <v>3</v>
       </c>
       <c r="U3" s="3" t="n">
-        <v>115.088107965157</v>
+        <v>522.679064980641</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>0.0201539066179668</v>
@@ -983,22 +984,22 @@
         <v>54</v>
       </c>
       <c r="AA3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="AB3" s="3" t="n">
-        <v>1070394963.8733</v>
+        <v>655305219518.846</v>
       </c>
       <c r="AC3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="AD3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="AE3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="AF3" s="1" t="n">
-        <v>0.587831152843765</v>
+        <v>0.755523981460554</v>
       </c>
       <c r="AG3" s="1" t="n">
         <v>0.145906279436112</v>
@@ -1007,16 +1008,16 @@
         <v>0.145906279436112</v>
       </c>
       <c r="AI3" s="1" t="n">
-        <v>0.110595627577536</v>
+        <v>0.299052545640919</v>
       </c>
       <c r="AJ3" s="1" t="n">
-        <v>0.110595627577536</v>
+        <v>0.299052545640919</v>
       </c>
       <c r="AK3" s="1" t="n">
-        <v>0.110595627577536</v>
+        <v>0.299052545640919</v>
       </c>
       <c r="AL3" s="1" t="n">
-        <v>0.110595627577536</v>
+        <v>0.299052545640919</v>
       </c>
       <c r="AN3" s="1" t="n">
         <v>0</v>
@@ -1039,40 +1040,40 @@
         <v>55</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="G4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="P4" s="1" t="n">
         <v>0</v>
@@ -1090,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="U4" s="3" t="n">
-        <v>128.85540779238</v>
+        <v>549.426120772896</v>
       </c>
       <c r="V4" s="1" t="n">
         <v>0.0254572989502525</v>
@@ -1108,22 +1109,22 @@
         <v>56</v>
       </c>
       <c r="AA4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="AB4" s="3" t="n">
-        <v>1205142276.13747</v>
+        <v>694710622753.651</v>
       </c>
       <c r="AC4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="AD4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="AE4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="AF4" s="1" t="n">
-        <v>0.612353705046949</v>
+        <v>0.794376802207163</v>
       </c>
       <c r="AG4" s="1" t="n">
         <v>0.165487544124068</v>
@@ -1132,16 +1133,16 @@
         <v>0.165487544124068</v>
       </c>
       <c r="AI4" s="1" t="n">
-        <v>0.123202810249796</v>
+        <v>0.317455850531352</v>
       </c>
       <c r="AJ4" s="1" t="n">
-        <v>0.123202810249796</v>
+        <v>0.317455850531352</v>
       </c>
       <c r="AK4" s="1" t="n">
-        <v>0.123202810249796</v>
+        <v>0.317455850531352</v>
       </c>
       <c r="AL4" s="1" t="n">
-        <v>0.123202810249796</v>
+        <v>0.317455850531352</v>
       </c>
       <c r="AN4" s="1" t="n">
         <v>0</v>
@@ -1164,40 +1165,40 @@
         <v>57</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="P5" s="1" t="n">
         <v>0</v>
@@ -1215,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="U5" s="3" t="n">
-        <v>144.269607094136</v>
+        <v>577.541903651207</v>
       </c>
       <c r="V5" s="1" t="n">
         <v>0.0321562505040478</v>
@@ -1233,22 +1234,22 @@
         <v>58</v>
       </c>
       <c r="AA5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="AB5" s="3" t="n">
-        <v>1356852334.6544</v>
+        <v>736485587160.634</v>
       </c>
       <c r="AC5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="AD5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="AE5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="AF5" s="1" t="n">
-        <v>0.637899264560392</v>
+        <v>0.835227629260666</v>
       </c>
       <c r="AG5" s="1" t="n">
         <v>0.187696700690712</v>
@@ -1257,16 +1258,16 @@
         <v>0.187696700690712</v>
       </c>
       <c r="AI5" s="1" t="n">
-        <v>0.137247129800006</v>
+        <v>0.336991670880446</v>
       </c>
       <c r="AJ5" s="1" t="n">
-        <v>0.137247129800006</v>
+        <v>0.336991670880446</v>
       </c>
       <c r="AK5" s="1" t="n">
-        <v>0.137247129800006</v>
+        <v>0.336991670880446</v>
       </c>
       <c r="AL5" s="1" t="n">
-        <v>0.137247129800006</v>
+        <v>0.336991670880446</v>
       </c>
       <c r="AN5" s="1" t="n">
         <v>0</v>
@@ -1289,40 +1290,40 @@
         <v>59</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="P6" s="1" t="n">
         <v>0</v>
@@ -1340,7 +1341,7 @@
         <v>8</v>
       </c>
       <c r="U6" s="3" t="n">
-        <v>161.527714573165</v>
+        <v>607.09645548675</v>
       </c>
       <c r="V6" s="1" t="n">
         <v>0.0406179951965728</v>
@@ -1358,22 +1359,22 @@
         <v>60</v>
       </c>
       <c r="AA6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="AB6" s="3" t="n">
-        <v>1527660504.91377</v>
+        <v>780772601324.805</v>
       </c>
       <c r="AC6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="AD6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="AE6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="AF6" s="1" t="n">
-        <v>0.664510508180058</v>
+        <v>0.878179210095396</v>
       </c>
       <c r="AG6" s="1" t="n">
         <v>0.212886423788889</v>
@@ -1382,16 +1383,16 @@
         <v>0.212886423788889</v>
       </c>
       <c r="AI6" s="1" t="n">
-        <v>0.152892410490863</v>
+        <v>0.357729700217256</v>
       </c>
       <c r="AJ6" s="1" t="n">
-        <v>0.152892410490863</v>
+        <v>0.357729700217256</v>
       </c>
       <c r="AK6" s="1" t="n">
-        <v>0.152892410490863</v>
+        <v>0.357729700217256</v>
       </c>
       <c r="AL6" s="1" t="n">
-        <v>0.152892410490863</v>
+        <v>0.357729700217256</v>
       </c>
       <c r="AN6" s="1" t="n">
         <v>0</v>
@@ -1414,40 +1415,40 @@
         <v>61</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="K7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="P7" s="1" t="n">
         <v>0</v>
@@ -1465,7 +1466,7 @@
         <v>6</v>
       </c>
       <c r="U7" s="3" t="n">
-        <v>180.850305901265</v>
+        <v>638.163402403374</v>
       </c>
       <c r="V7" s="1" t="n">
         <v>0.0513064025789055</v>
@@ -1483,22 +1484,22 @@
         <v>62</v>
       </c>
       <c r="AA7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="AB7" s="3" t="n">
-        <v>1719970964.17115</v>
+        <v>827722722083.01</v>
       </c>
       <c r="AC7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="AD7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="AE7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="AF7" s="1" t="n">
-        <v>0.692231893049806</v>
+        <v>0.923339575974552</v>
       </c>
       <c r="AG7" s="1" t="n">
         <v>0.241456718561622</v>
@@ -1507,16 +1508,16 @@
         <v>0.241456718561622</v>
       </c>
       <c r="AI7" s="1" t="n">
-        <v>0.170321151486153</v>
+        <v>0.379743920920016</v>
       </c>
       <c r="AJ7" s="1" t="n">
-        <v>0.170321151486153</v>
+        <v>0.379743920920016</v>
       </c>
       <c r="AK7" s="1" t="n">
-        <v>0.170321151486153</v>
+        <v>0.379743920920016</v>
       </c>
       <c r="AL7" s="1" t="n">
-        <v>0.170321151486153</v>
+        <v>0.379743920920016</v>
       </c>
       <c r="AN7" s="1" t="n">
         <v>0</v>
@@ -1539,40 +1540,40 @@
         <v>63</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="M8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="P8" s="1" t="n">
         <v>0</v>
@@ -1590,7 +1591,7 @@
         <v>5</v>
       </c>
       <c r="U8" s="3" t="n">
-        <v>202.484342894398</v>
+        <v>670.820138194562</v>
       </c>
       <c r="V8" s="1" t="n">
         <v>0.0648074069842528</v>
@@ -1608,22 +1609,22 @@
         <v>64</v>
       </c>
       <c r="AA8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="AB8" s="3" t="n">
-        <v>1936490540.97841</v>
+        <v>877496089757.755</v>
       </c>
       <c r="AC8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="AD8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="AE8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="AF8" s="1" t="n">
-        <v>0.721109730932165</v>
+        <v>0.970822313669044</v>
       </c>
       <c r="AG8" s="1" t="n">
         <v>0.273861272602154</v>
@@ -1632,16 +1633,16 @@
         <v>0.273861272602154</v>
       </c>
       <c r="AI8" s="1" t="n">
-        <v>0.18973665566809</v>
+        <v>0.403112868146337</v>
       </c>
       <c r="AJ8" s="1" t="n">
-        <v>0.18973665566809</v>
+        <v>0.403112868146337</v>
       </c>
       <c r="AK8" s="1" t="n">
-        <v>0.18973665566809</v>
+        <v>0.403112868146337</v>
       </c>
       <c r="AL8" s="1" t="n">
-        <v>0.18973665566809</v>
+        <v>0.403112868146337</v>
       </c>
       <c r="AM8" s="1" t="s">
         <v>65</v>
@@ -1667,40 +1668,40 @@
         <v>66</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>0</v>
@@ -1718,7 +1719,7 @@
         <v>8</v>
       </c>
       <c r="U9" s="3" t="n">
-        <v>226.706329928798</v>
+        <v>705.148017126392</v>
       </c>
       <c r="V9" s="1" t="n">
         <v>0.0818611282200753</v>
@@ -1736,22 +1737,22 @@
         <v>67</v>
       </c>
       <c r="AA9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="AB9" s="3" t="n">
-        <v>2180266814.6238</v>
+        <v>930262474373.549</v>
       </c>
       <c r="AC9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="AD9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="AE9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="AF9" s="1" t="n">
-        <v>0.751192265577462</v>
+        <v>1.02074685114947</v>
       </c>
       <c r="AG9" s="1" t="n">
         <v>0.310614660374962</v>
@@ -1760,16 +1761,16 @@
         <v>0.310614660374962</v>
       </c>
       <c r="AI9" s="1" t="n">
-        <v>0.21136540112599</v>
+        <v>0.427919910005334</v>
       </c>
       <c r="AJ9" s="1" t="n">
-        <v>0.21136540112599</v>
+        <v>0.427919910005334</v>
       </c>
       <c r="AK9" s="1" t="n">
-        <v>0.21136540112599</v>
+        <v>0.427919910005334</v>
       </c>
       <c r="AL9" s="1" t="n">
-        <v>0.21136540112599</v>
+        <v>0.427919910005334</v>
       </c>
       <c r="AN9" s="1" t="n">
         <v>0</v>
@@ -1792,40 +1793,40 @@
         <v>68</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="J10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="K10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="P10" s="1" t="n">
         <v>0</v>
@@ -1843,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="U10" s="3" t="n">
-        <v>253.8258479402</v>
+        <v>741.232556606801</v>
       </c>
       <c r="V10" s="1" t="n">
         <v>0.103402444647907</v>
@@ -1861,22 +1862,22 @@
         <v>69</v>
       </c>
       <c r="AA10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="AB10" s="3" t="n">
-        <v>2454731010.74281</v>
+        <v>986201854718.806</v>
       </c>
       <c r="AC10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="AD10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="AE10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="AF10" s="1" t="n">
-        <v>0.782529753320557</v>
+        <v>1.07323875796984</v>
       </c>
       <c r="AG10" s="1" t="n">
         <v>0.352300514501788</v>
@@ -1885,16 +1886,16 @@
         <v>0.352300514501788</v>
       </c>
       <c r="AI10" s="1" t="n">
-        <v>0.235459682979246</v>
+        <v>0.454253544971179</v>
       </c>
       <c r="AJ10" s="1" t="n">
-        <v>0.235459682979246</v>
+        <v>0.454253544971179</v>
       </c>
       <c r="AK10" s="1" t="n">
-        <v>0.235459682979246</v>
+        <v>0.454253544971179</v>
       </c>
       <c r="AL10" s="1" t="n">
-        <v>0.235459682979246</v>
+        <v>0.454253544971179</v>
       </c>
       <c r="AN10" s="1" t="n">
         <v>0</v>
@@ -1917,40 +1918,40 @@
         <v>70</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="P11" s="1" t="n">
         <v>0</v>
@@ -1968,7 +1969,7 @@
         <v>4</v>
       </c>
       <c r="U11" s="3" t="n">
-        <v>284.189511174199</v>
+        <v>779.16365022604</v>
       </c>
       <c r="V11" s="1" t="n">
         <v>0.13061224285132</v>
@@ -1986,22 +1987,22 @@
         <v>71</v>
       </c>
       <c r="AA11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="AB11" s="3" t="n">
-        <v>2763746296.86877</v>
+        <v>1045505032228.43</v>
       </c>
       <c r="AC11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="AD11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="AE11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="AF11" s="1" t="n">
-        <v>0.81517454703983</v>
+        <v>1.12843006109843</v>
       </c>
       <c r="AG11" s="1" t="n">
         <v>0.399580793670191</v>
@@ -2010,16 +2011,16 @@
         <v>0.399580793670191</v>
       </c>
       <c r="AI11" s="1" t="n">
-        <v>0.262300556350941</v>
+        <v>0.482207717599097</v>
       </c>
       <c r="AJ11" s="1" t="n">
-        <v>0.262300556350941</v>
+        <v>0.482207717599097</v>
       </c>
       <c r="AK11" s="1" t="n">
-        <v>0.262300556350941</v>
+        <v>0.482207717599097</v>
       </c>
       <c r="AL11" s="1" t="n">
-        <v>0.262300556350941</v>
+        <v>0.482207717599097</v>
       </c>
       <c r="AN11" s="1" t="n">
         <v>0</v>
@@ -2042,40 +2043,40 @@
         <v>72</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="L12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="P12" s="1" t="n">
         <v>0</v>
@@ -2093,7 +2094,7 @@
         <v>3</v>
       </c>
       <c r="U12" s="3" t="n">
-        <v>318.185397258901</v>
+        <v>819.035791699057</v>
       </c>
       <c r="V12" s="1" t="n">
         <v>0.164982153378881</v>
@@ -2111,22 +2112,22 @@
         <v>73</v>
       </c>
       <c r="AA12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="AB12" s="3" t="n">
-        <v>3111662157.69788</v>
+        <v>1108374281780.92</v>
       </c>
       <c r="AC12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="AD12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="AE12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="AF12" s="1" t="n">
-        <v>0.849181183618691</v>
+        <v>1.18645957699042</v>
       </c>
       <c r="AG12" s="1" t="n">
         <v>0.453206294336223</v>
@@ -2135,16 +2136,16 @@
         <v>0.453206294336223</v>
       </c>
       <c r="AI12" s="1" t="n">
-        <v>0.292201114821332</v>
+        <v>0.511882153670112</v>
       </c>
       <c r="AJ12" s="1" t="n">
-        <v>0.292201114821332</v>
+        <v>0.511882153670112</v>
       </c>
       <c r="AK12" s="1" t="n">
-        <v>0.292201114821332</v>
+        <v>0.511882153670112</v>
       </c>
       <c r="AL12" s="1" t="n">
-        <v>0.292201114821332</v>
+        <v>0.511882153670112</v>
       </c>
       <c r="AM12" s="1" t="s">
         <v>74</v>
@@ -2170,40 +2171,40 @@
         <v>75</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="P13" s="1" t="n">
         <v>0</v>
@@ -2221,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="U13" s="3" t="n">
-        <v>356.2480072206</v>
+        <v>860.948310267673</v>
       </c>
       <c r="V13" s="1" t="n">
         <v>0.208396321350341</v>
@@ -2239,22 +2240,22 @@
         <v>76</v>
       </c>
       <c r="AA13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="AB13" s="3" t="n">
-        <v>3503375615.41697</v>
+        <v>1175024041629.82</v>
       </c>
       <c r="AC13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="AD13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="AE13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="AF13" s="1" t="n">
-        <v>0.884606475055712</v>
+        <v>1.24747326073715</v>
       </c>
       <c r="AG13" s="1" t="n">
         <v>0.514028573143839</v>
@@ -2263,16 +2264,16 @@
         <v>0.514028573143839</v>
       </c>
       <c r="AI13" s="1" t="n">
-        <v>0.325510142603717</v>
+        <v>0.543382715960171</v>
       </c>
       <c r="AJ13" s="1" t="n">
-        <v>0.325510142603717</v>
+        <v>0.543382715960171</v>
       </c>
       <c r="AK13" s="1" t="n">
-        <v>0.325510142603717</v>
+        <v>0.543382715960171</v>
       </c>
       <c r="AL13" s="1" t="n">
-        <v>0.325510142603717</v>
+        <v>0.543382715960171</v>
       </c>
       <c r="AN13" s="1" t="n">
         <v>0</v>
@@ -2295,40 +2296,40 @@
         <v>77</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="P14" s="1" t="n">
         <v>0</v>
@@ -2346,7 +2347,7 @@
         <v>7</v>
       </c>
       <c r="U14" s="3" t="n">
-        <v>398.863818836357</v>
+        <v>905.005618149001</v>
       </c>
       <c r="V14" s="1" t="n">
         <v>0.263234694558872</v>
@@ -2364,22 +2365,22 @@
         <v>78</v>
       </c>
       <c r="AA14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="AB14" s="3" t="n">
-        <v>3944400156.7891</v>
+        <v>1245681644822.74</v>
       </c>
       <c r="AC14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="AD14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="AE14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="AF14" s="1" t="n">
-        <v>0.921509603375611</v>
+        <v>1.31162457317056</v>
       </c>
       <c r="AG14" s="1" t="n">
         <v>0.583013469385465</v>
@@ -2388,16 +2389,16 @@
         <v>0.583013469385465</v>
       </c>
       <c r="AI14" s="1" t="n">
-        <v>0.362616183044614</v>
+        <v>0.57682178190283</v>
       </c>
       <c r="AJ14" s="1" t="n">
-        <v>0.362616183044614</v>
+        <v>0.57682178190283</v>
       </c>
       <c r="AK14" s="1" t="n">
-        <v>0.362616183044614</v>
+        <v>0.57682178190283</v>
       </c>
       <c r="AL14" s="1" t="n">
-        <v>0.362616183044614</v>
+        <v>0.57682178190283</v>
       </c>
       <c r="AN14" s="1" t="n">
         <v>0</v>
@@ -2420,40 +2421,40 @@
         <v>79</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="P15" s="1" t="n">
         <v>0</v>
@@ -2471,7 +2472,7 @@
         <v>8</v>
       </c>
       <c r="U15" s="3" t="n">
-        <v>446.577504300838</v>
+        <v>951.31747064654</v>
       </c>
       <c r="V15" s="1" t="n">
         <v>0.332503491282904</v>
@@ -2489,22 +2490,22 @@
         <v>80</v>
       </c>
       <c r="AA15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="AB15" s="3" t="n">
-        <v>4440943337.16659</v>
+        <v>1320588094602.7</v>
       </c>
       <c r="AC15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="AD15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="AE15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="AF15" s="1" t="n">
-        <v>0.959952219499631</v>
+        <v>1.37907486684586</v>
       </c>
       <c r="AG15" s="1" t="n">
         <v>0.661256442236259</v>
@@ -2513,16 +2514,16 @@
         <v>0.661256442236259</v>
       </c>
       <c r="AI15" s="1" t="n">
-        <v>0.40395207090651</v>
+        <v>0.612318644492813</v>
       </c>
       <c r="AJ15" s="1" t="n">
-        <v>0.40395207090651</v>
+        <v>0.612318644492813</v>
       </c>
       <c r="AK15" s="1" t="n">
-        <v>0.40395207090651</v>
+        <v>0.612318644492813</v>
       </c>
       <c r="AL15" s="1" t="n">
-        <v>0.40395207090651</v>
+        <v>0.612318644492813</v>
       </c>
       <c r="AN15" s="1" t="n">
         <v>0</v>
@@ -2545,40 +2546,40 @@
         <v>81</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="G16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="H16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="I16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="J16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="L16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="P16" s="1" t="n">
         <v>0</v>
@@ -2596,7 +2597,7 @@
         <v>6</v>
       </c>
       <c r="U16" s="3" t="n">
-        <v>499.998891675321</v>
+        <v>999.999239571935</v>
       </c>
       <c r="V16" s="1" t="n">
         <v>0.420000000002258</v>
@@ -2614,22 +2615,22 @@
         <v>82</v>
       </c>
       <c r="AA16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="AB16" s="3" t="n">
-        <v>4999994153.73181</v>
+        <v>1399998886436.64</v>
       </c>
       <c r="AC16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="AD16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="AE16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="AF16" s="1" t="n">
-        <v>0.999998546240497</v>
+        <v>1.44999379187341</v>
       </c>
       <c r="AG16" s="1" t="n">
         <v>0.749999966312711</v>
@@ -2638,16 +2639,16 @@
         <v>0.749999966312711</v>
       </c>
       <c r="AI16" s="1" t="n">
-        <v>0.449999981301391</v>
+        <v>0.649999937860663</v>
       </c>
       <c r="AJ16" s="1" t="n">
-        <v>0.449999981301391</v>
+        <v>0.649999937860663</v>
       </c>
       <c r="AK16" s="1" t="n">
-        <v>0.449999981301391</v>
+        <v>0.649999937860663</v>
       </c>
       <c r="AL16" s="1" t="n">
-        <v>0.449999981301391</v>
+        <v>0.649999937860663</v>
       </c>
       <c r="AM16" s="5" t="s">
         <v>83</v>

</xml_diff>